<commit_message>
Cải thiện và tối ưu thuật toán GA cho quy trình tạo thời khoá biểu
</commit_message>
<xml_diff>
--- a/timetabling_GA/results/HK1_CT02/TKB_HocKy_GiangVien.xlsx
+++ b/timetabling_GA/results/HK1_CT02/TKB_HocKy_GiangVien.xlsx
@@ -84,14 +84,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00BDD7EE"/>
-        <bgColor rgb="00BDD7EE"/>
+        <fgColor rgb="00FFE699"/>
+        <bgColor rgb="00FFE699"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFE699"/>
-        <bgColor rgb="00FFE699"/>
+        <fgColor rgb="00BDD7EE"/>
+        <bgColor rgb="00BDD7EE"/>
       </patternFill>
     </fill>
   </fills>
@@ -121,7 +121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -150,6 +150,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -515,7 +516,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -607,8 +608,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C1
-(13:00-15:00)</t>
+          <t>S1
+(07:00-09:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -616,16 +617,16 @@
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C8" s="7" t="inlineStr"/>
+      <c r="C8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
       <c r="D8" s="7" t="inlineStr"/>
-      <c r="E8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
@@ -633,61 +634,117 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
+          <t>S2
+(09:00-11:00)</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>Trần Thị B</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="inlineStr"/>
+      <c r="D9" s="7" t="inlineStr"/>
+      <c r="E9" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="7" t="inlineStr"/>
+      <c r="H9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="10" t="n"/>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="inlineStr"/>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="G10" s="7" t="inlineStr"/>
+      <c r="H10" s="7" t="inlineStr"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
           <t>C2
 (15:00-17:00)</t>
         </is>
       </c>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>Phạm Văn D</t>
-        </is>
-      </c>
-      <c r="C9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
-      <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
-    </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>T2
-(19:30-21:30)</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
+      <c r="B11" s="7" t="inlineStr">
         <is>
           <t>Trần Thị B</t>
         </is>
       </c>
-      <c r="C10" s="7" t="inlineStr"/>
-      <c r="D10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: LAB01
-(Thực hành)</t>
-        </is>
-      </c>
-      <c r="E10" s="7" t="inlineStr"/>
-      <c r="F10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: LAB04
-(Thực hành)</t>
-        </is>
-      </c>
-      <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
+      <c r="C11" s="7" t="inlineStr"/>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+      <c r="G11" s="7" t="inlineStr"/>
+      <c r="H11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="n"/>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="inlineStr"/>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="F12" s="7" t="inlineStr"/>
+      <c r="G12" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+      <c r="H12" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -706,7 +763,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -798,8 +855,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C1
-(13:00-15:00)</t>
+          <t>S1
+(07:00-09:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -807,16 +864,16 @@
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C8" s="7" t="inlineStr"/>
+      <c r="C8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
       <c r="D8" s="7" t="inlineStr"/>
-      <c r="E8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
@@ -824,61 +881,117 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
+          <t>S2
+(09:00-11:00)</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>Trần Thị B</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="inlineStr"/>
+      <c r="D9" s="7" t="inlineStr"/>
+      <c r="E9" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="7" t="inlineStr"/>
+      <c r="H9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="10" t="n"/>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="inlineStr"/>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="G10" s="7" t="inlineStr"/>
+      <c r="H10" s="7" t="inlineStr"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
           <t>C2
 (15:00-17:00)</t>
         </is>
       </c>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>Phạm Văn D</t>
-        </is>
-      </c>
-      <c r="C9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
-      <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
-    </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>T2
-(19:30-21:30)</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
+      <c r="B11" s="7" t="inlineStr">
         <is>
           <t>Trần Thị B</t>
         </is>
       </c>
-      <c r="C10" s="7" t="inlineStr"/>
-      <c r="D10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: LAB01
-(Thực hành)</t>
-        </is>
-      </c>
-      <c r="E10" s="7" t="inlineStr"/>
-      <c r="F10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: LAB04
-(Thực hành)</t>
-        </is>
-      </c>
-      <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
+      <c r="C11" s="7" t="inlineStr"/>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+      <c r="G11" s="7" t="inlineStr"/>
+      <c r="H11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="n"/>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="inlineStr"/>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="F12" s="7" t="inlineStr"/>
+      <c r="G12" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+      <c r="H12" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -897,7 +1010,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -989,8 +1102,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C1
-(13:00-15:00)</t>
+          <t>S1
+(07:00-09:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -998,16 +1111,16 @@
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C8" s="7" t="inlineStr"/>
+      <c r="C8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
       <c r="D8" s="7" t="inlineStr"/>
-      <c r="E8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
@@ -1015,61 +1128,117 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
+          <t>S2
+(09:00-11:00)</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>Trần Thị B</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="inlineStr"/>
+      <c r="D9" s="7" t="inlineStr"/>
+      <c r="E9" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="7" t="inlineStr"/>
+      <c r="H9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="10" t="n"/>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="inlineStr"/>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="G10" s="7" t="inlineStr"/>
+      <c r="H10" s="7" t="inlineStr"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
           <t>C2
 (15:00-17:00)</t>
         </is>
       </c>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>Phạm Văn D</t>
-        </is>
-      </c>
-      <c r="C9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
-      <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
-    </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>T2
-(19:30-21:30)</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
+      <c r="B11" s="7" t="inlineStr">
         <is>
           <t>Trần Thị B</t>
         </is>
       </c>
-      <c r="C10" s="7" t="inlineStr"/>
-      <c r="D10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: LAB01
-(Thực hành)</t>
-        </is>
-      </c>
-      <c r="E10" s="7" t="inlineStr"/>
-      <c r="F10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: LAB04
-(Thực hành)</t>
-        </is>
-      </c>
-      <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
+      <c r="C11" s="7" t="inlineStr"/>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+      <c r="G11" s="7" t="inlineStr"/>
+      <c r="H11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="n"/>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="inlineStr"/>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="F12" s="7" t="inlineStr"/>
+      <c r="G12" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+      <c r="H12" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1088,7 +1257,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1180,8 +1349,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C1
-(13:00-15:00)</t>
+          <t>S1
+(07:00-09:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -1189,16 +1358,16 @@
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C8" s="7" t="inlineStr"/>
+      <c r="C8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
       <c r="D8" s="7" t="inlineStr"/>
-      <c r="E8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
@@ -1206,61 +1375,117 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
+          <t>S2
+(09:00-11:00)</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>Trần Thị B</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="inlineStr"/>
+      <c r="D9" s="7" t="inlineStr"/>
+      <c r="E9" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="7" t="inlineStr"/>
+      <c r="H9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="10" t="n"/>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="inlineStr"/>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="G10" s="7" t="inlineStr"/>
+      <c r="H10" s="7" t="inlineStr"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
           <t>C2
 (15:00-17:00)</t>
         </is>
       </c>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>Phạm Văn D</t>
-        </is>
-      </c>
-      <c r="C9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
-      <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
-    </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>T2
-(19:30-21:30)</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
+      <c r="B11" s="7" t="inlineStr">
         <is>
           <t>Trần Thị B</t>
         </is>
       </c>
-      <c r="C10" s="7" t="inlineStr"/>
-      <c r="D10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: LAB01
-(Thực hành)</t>
-        </is>
-      </c>
-      <c r="E10" s="7" t="inlineStr"/>
-      <c r="F10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: LAB04
-(Thực hành)</t>
-        </is>
-      </c>
-      <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
+      <c r="C11" s="7" t="inlineStr"/>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+      <c r="G11" s="7" t="inlineStr"/>
+      <c r="H11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="n"/>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="inlineStr"/>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="F12" s="7" t="inlineStr"/>
+      <c r="G12" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+      <c r="H12" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1279,7 +1504,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1371,8 +1596,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C1
-(13:00-15:00)</t>
+          <t>S1
+(07:00-09:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -1380,16 +1605,16 @@
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C8" s="7" t="inlineStr"/>
+      <c r="C8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
       <c r="D8" s="7" t="inlineStr"/>
-      <c r="E8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
@@ -1397,61 +1622,117 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
+          <t>S2
+(09:00-11:00)</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>Trần Thị B</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="inlineStr"/>
+      <c r="D9" s="7" t="inlineStr"/>
+      <c r="E9" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="7" t="inlineStr"/>
+      <c r="H9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="10" t="n"/>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="inlineStr"/>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="G10" s="7" t="inlineStr"/>
+      <c r="H10" s="7" t="inlineStr"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
           <t>C2
 (15:00-17:00)</t>
         </is>
       </c>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>Phạm Văn D</t>
-        </is>
-      </c>
-      <c r="C9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
-      <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
-    </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>T2
-(19:30-21:30)</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
+      <c r="B11" s="7" t="inlineStr">
         <is>
           <t>Trần Thị B</t>
         </is>
       </c>
-      <c r="C10" s="7" t="inlineStr"/>
-      <c r="D10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: LAB01
-(Thực hành)</t>
-        </is>
-      </c>
-      <c r="E10" s="7" t="inlineStr"/>
-      <c r="F10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: LAB04
-(Thực hành)</t>
-        </is>
-      </c>
-      <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
+      <c r="C11" s="7" t="inlineStr"/>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+      <c r="G11" s="7" t="inlineStr"/>
+      <c r="H11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="n"/>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="inlineStr"/>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="F12" s="7" t="inlineStr"/>
+      <c r="G12" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+      <c r="H12" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1470,7 +1751,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1562,8 +1843,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C1
-(13:00-15:00)</t>
+          <t>S1
+(07:00-09:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -1571,16 +1852,16 @@
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C8" s="7" t="inlineStr"/>
+      <c r="C8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
       <c r="D8" s="7" t="inlineStr"/>
-      <c r="E8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
@@ -1588,61 +1869,117 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
+          <t>S2
+(09:00-11:00)</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>Trần Thị B</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="inlineStr"/>
+      <c r="D9" s="7" t="inlineStr"/>
+      <c r="E9" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="7" t="inlineStr"/>
+      <c r="H9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="10" t="n"/>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="inlineStr"/>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="G10" s="7" t="inlineStr"/>
+      <c r="H10" s="7" t="inlineStr"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
           <t>C2
 (15:00-17:00)</t>
         </is>
       </c>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>Phạm Văn D</t>
-        </is>
-      </c>
-      <c r="C9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
-      <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
-    </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>T2
-(19:30-21:30)</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
+      <c r="B11" s="7" t="inlineStr">
         <is>
           <t>Trần Thị B</t>
         </is>
       </c>
-      <c r="C10" s="7" t="inlineStr"/>
-      <c r="D10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: LAB01
-(Thực hành)</t>
-        </is>
-      </c>
-      <c r="E10" s="7" t="inlineStr"/>
-      <c r="F10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: LAB04
-(Thực hành)</t>
-        </is>
-      </c>
-      <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
+      <c r="C11" s="7" t="inlineStr"/>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+      <c r="G11" s="7" t="inlineStr"/>
+      <c r="H11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="n"/>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="inlineStr"/>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="F12" s="7" t="inlineStr"/>
+      <c r="G12" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+      <c r="H12" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1661,7 +1998,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1753,8 +2090,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C1
-(13:00-15:00)</t>
+          <t>S1
+(07:00-09:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -1762,16 +2099,16 @@
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C8" s="7" t="inlineStr"/>
+      <c r="C8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
       <c r="D8" s="7" t="inlineStr"/>
-      <c r="E8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
@@ -1779,61 +2116,117 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
+          <t>S2
+(09:00-11:00)</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>Trần Thị B</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="inlineStr"/>
+      <c r="D9" s="7" t="inlineStr"/>
+      <c r="E9" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="7" t="inlineStr"/>
+      <c r="H9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="10" t="n"/>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="inlineStr"/>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="G10" s="7" t="inlineStr"/>
+      <c r="H10" s="7" t="inlineStr"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
           <t>C2
 (15:00-17:00)</t>
         </is>
       </c>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>Phạm Văn D</t>
-        </is>
-      </c>
-      <c r="C9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
-      <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
-    </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>T2
-(19:30-21:30)</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
+      <c r="B11" s="7" t="inlineStr">
         <is>
           <t>Trần Thị B</t>
         </is>
       </c>
-      <c r="C10" s="7" t="inlineStr"/>
-      <c r="D10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: LAB01
-(Thực hành)</t>
-        </is>
-      </c>
-      <c r="E10" s="7" t="inlineStr"/>
-      <c r="F10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: LAB04
-(Thực hành)</t>
-        </is>
-      </c>
-      <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
+      <c r="C11" s="7" t="inlineStr"/>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+      <c r="G11" s="7" t="inlineStr"/>
+      <c r="H11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="n"/>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="inlineStr"/>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="F12" s="7" t="inlineStr"/>
+      <c r="G12" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+      <c r="H12" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1852,7 +2245,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1944,8 +2337,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C1
-(13:00-15:00)</t>
+          <t>S1
+(07:00-09:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -1953,16 +2346,16 @@
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C8" s="7" t="inlineStr"/>
+      <c r="C8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
       <c r="D8" s="7" t="inlineStr"/>
-      <c r="E8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
@@ -1970,61 +2363,117 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
+          <t>S2
+(09:00-11:00)</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>Trần Thị B</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="inlineStr"/>
+      <c r="D9" s="7" t="inlineStr"/>
+      <c r="E9" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="7" t="inlineStr"/>
+      <c r="H9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="10" t="n"/>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="inlineStr"/>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="G10" s="7" t="inlineStr"/>
+      <c r="H10" s="7" t="inlineStr"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
           <t>C2
 (15:00-17:00)</t>
         </is>
       </c>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>Phạm Văn D</t>
-        </is>
-      </c>
-      <c r="C9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
-      <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
-    </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>T2
-(19:30-21:30)</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
+      <c r="B11" s="7" t="inlineStr">
         <is>
           <t>Trần Thị B</t>
         </is>
       </c>
-      <c r="C10" s="7" t="inlineStr"/>
-      <c r="D10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: LAB01
-(Thực hành)</t>
-        </is>
-      </c>
-      <c r="E10" s="7" t="inlineStr"/>
-      <c r="F10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: LAB04
-(Thực hành)</t>
-        </is>
-      </c>
-      <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
+      <c r="C11" s="7" t="inlineStr"/>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+      <c r="G11" s="7" t="inlineStr"/>
+      <c r="H11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="n"/>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="inlineStr"/>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="F12" s="7" t="inlineStr"/>
+      <c r="G12" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+      <c r="H12" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2043,7 +2492,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2135,8 +2584,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C1
-(13:00-15:00)</t>
+          <t>S1
+(07:00-09:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -2144,16 +2593,16 @@
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C8" s="7" t="inlineStr"/>
+      <c r="C8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
       <c r="D8" s="7" t="inlineStr"/>
-      <c r="E8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
@@ -2161,61 +2610,117 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
+          <t>S2
+(09:00-11:00)</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>Trần Thị B</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="inlineStr"/>
+      <c r="D9" s="7" t="inlineStr"/>
+      <c r="E9" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="7" t="inlineStr"/>
+      <c r="H9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="10" t="n"/>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="inlineStr"/>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="G10" s="7" t="inlineStr"/>
+      <c r="H10" s="7" t="inlineStr"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
           <t>C2
 (15:00-17:00)</t>
         </is>
       </c>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>Phạm Văn D</t>
-        </is>
-      </c>
-      <c r="C9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
-      <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
-    </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>T2
-(19:30-21:30)</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
+      <c r="B11" s="7" t="inlineStr">
         <is>
           <t>Trần Thị B</t>
         </is>
       </c>
-      <c r="C10" s="7" t="inlineStr"/>
-      <c r="D10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: LAB01
-(Thực hành)</t>
-        </is>
-      </c>
-      <c r="E10" s="7" t="inlineStr"/>
-      <c r="F10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: LAB04
-(Thực hành)</t>
-        </is>
-      </c>
-      <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
+      <c r="C11" s="7" t="inlineStr"/>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+      <c r="G11" s="7" t="inlineStr"/>
+      <c r="H11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="n"/>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="inlineStr"/>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="F12" s="7" t="inlineStr"/>
+      <c r="G12" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+      <c r="H12" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2234,7 +2739,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2326,8 +2831,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C1
-(13:00-15:00)</t>
+          <t>S1
+(07:00-09:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -2335,16 +2840,16 @@
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C8" s="7" t="inlineStr"/>
+      <c r="C8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
       <c r="D8" s="7" t="inlineStr"/>
-      <c r="E8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
@@ -2352,61 +2857,117 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
+          <t>S2
+(09:00-11:00)</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>Trần Thị B</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="inlineStr"/>
+      <c r="D9" s="7" t="inlineStr"/>
+      <c r="E9" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="7" t="inlineStr"/>
+      <c r="H9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="10" t="n"/>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="inlineStr"/>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="G10" s="7" t="inlineStr"/>
+      <c r="H10" s="7" t="inlineStr"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
           <t>C2
 (15:00-17:00)</t>
         </is>
       </c>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>Phạm Văn D</t>
-        </is>
-      </c>
-      <c r="C9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
-      <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
-    </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>T2
-(19:30-21:30)</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
+      <c r="B11" s="7" t="inlineStr">
         <is>
           <t>Trần Thị B</t>
         </is>
       </c>
-      <c r="C10" s="7" t="inlineStr"/>
-      <c r="D10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: LAB01
-(Thực hành)</t>
-        </is>
-      </c>
-      <c r="E10" s="7" t="inlineStr"/>
-      <c r="F10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: LAB04
-(Thực hành)</t>
-        </is>
-      </c>
-      <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
+      <c r="C11" s="7" t="inlineStr"/>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+      <c r="G11" s="7" t="inlineStr"/>
+      <c r="H11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="n"/>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="inlineStr"/>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="F12" s="7" t="inlineStr"/>
+      <c r="G12" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+      <c r="H12" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2425,7 +2986,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2517,8 +3078,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C1
-(13:00-15:00)</t>
+          <t>S1
+(07:00-09:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -2526,16 +3087,16 @@
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C8" s="7" t="inlineStr"/>
+      <c r="C8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
       <c r="D8" s="7" t="inlineStr"/>
-      <c r="E8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
@@ -2543,61 +3104,117 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
+          <t>S2
+(09:00-11:00)</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>Trần Thị B</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="inlineStr"/>
+      <c r="D9" s="7" t="inlineStr"/>
+      <c r="E9" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="7" t="inlineStr"/>
+      <c r="H9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="10" t="n"/>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="inlineStr"/>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="G10" s="7" t="inlineStr"/>
+      <c r="H10" s="7" t="inlineStr"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
           <t>C2
 (15:00-17:00)</t>
         </is>
       </c>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>Phạm Văn D</t>
-        </is>
-      </c>
-      <c r="C9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
-      <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
-    </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>T2
-(19:30-21:30)</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
+      <c r="B11" s="7" t="inlineStr">
         <is>
           <t>Trần Thị B</t>
         </is>
       </c>
-      <c r="C10" s="7" t="inlineStr"/>
-      <c r="D10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: LAB01
-(Thực hành)</t>
-        </is>
-      </c>
-      <c r="E10" s="7" t="inlineStr"/>
-      <c r="F10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: LAB04
-(Thực hành)</t>
-        </is>
-      </c>
-      <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
+      <c r="C11" s="7" t="inlineStr"/>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+      <c r="G11" s="7" t="inlineStr"/>
+      <c r="H11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="n"/>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="inlineStr"/>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="F12" s="7" t="inlineStr"/>
+      <c r="G12" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+      <c r="H12" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2616,7 +3233,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2708,8 +3325,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C1
-(13:00-15:00)</t>
+          <t>S1
+(07:00-09:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -2717,16 +3334,16 @@
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C8" s="7" t="inlineStr"/>
+      <c r="C8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
       <c r="D8" s="7" t="inlineStr"/>
-      <c r="E8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
@@ -2734,61 +3351,117 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
+          <t>S2
+(09:00-11:00)</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>Trần Thị B</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="inlineStr"/>
+      <c r="D9" s="7" t="inlineStr"/>
+      <c r="E9" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="7" t="inlineStr"/>
+      <c r="H9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="10" t="n"/>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="inlineStr"/>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="G10" s="7" t="inlineStr"/>
+      <c r="H10" s="7" t="inlineStr"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
           <t>C2
 (15:00-17:00)</t>
         </is>
       </c>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>Phạm Văn D</t>
-        </is>
-      </c>
-      <c r="C9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
-      <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
-    </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>T2
-(19:30-21:30)</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
+      <c r="B11" s="7" t="inlineStr">
         <is>
           <t>Trần Thị B</t>
         </is>
       </c>
-      <c r="C10" s="7" t="inlineStr"/>
-      <c r="D10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: LAB01
-(Thực hành)</t>
-        </is>
-      </c>
-      <c r="E10" s="7" t="inlineStr"/>
-      <c r="F10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: LAB04
-(Thực hành)</t>
-        </is>
-      </c>
-      <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
+      <c r="C11" s="7" t="inlineStr"/>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+      <c r="G11" s="7" t="inlineStr"/>
+      <c r="H11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="n"/>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="inlineStr"/>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="F12" s="7" t="inlineStr"/>
+      <c r="G12" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+      <c r="H12" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2807,7 +3480,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2899,8 +3572,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C1
-(13:00-15:00)</t>
+          <t>S1
+(07:00-09:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -2908,16 +3581,16 @@
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C8" s="7" t="inlineStr"/>
+      <c r="C8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
       <c r="D8" s="7" t="inlineStr"/>
-      <c r="E8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
@@ -2925,61 +3598,117 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
+          <t>S2
+(09:00-11:00)</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>Trần Thị B</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="inlineStr"/>
+      <c r="D9" s="7" t="inlineStr"/>
+      <c r="E9" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="7" t="inlineStr"/>
+      <c r="H9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="10" t="n"/>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="inlineStr"/>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="G10" s="7" t="inlineStr"/>
+      <c r="H10" s="7" t="inlineStr"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
           <t>C2
 (15:00-17:00)</t>
         </is>
       </c>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>Phạm Văn D</t>
-        </is>
-      </c>
-      <c r="C9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
-      <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
-    </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>T2
-(19:30-21:30)</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
+      <c r="B11" s="7" t="inlineStr">
         <is>
           <t>Trần Thị B</t>
         </is>
       </c>
-      <c r="C10" s="7" t="inlineStr"/>
-      <c r="D10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: LAB01
-(Thực hành)</t>
-        </is>
-      </c>
-      <c r="E10" s="7" t="inlineStr"/>
-      <c r="F10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: LAB04
-(Thực hành)</t>
-        </is>
-      </c>
-      <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
+      <c r="C11" s="7" t="inlineStr"/>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+      <c r="G11" s="7" t="inlineStr"/>
+      <c r="H11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="n"/>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="inlineStr"/>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="F12" s="7" t="inlineStr"/>
+      <c r="G12" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+      <c r="H12" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2998,7 +3727,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3090,8 +3819,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C1
-(13:00-15:00)</t>
+          <t>S1
+(07:00-09:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -3099,16 +3828,16 @@
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C8" s="7" t="inlineStr"/>
+      <c r="C8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
       <c r="D8" s="7" t="inlineStr"/>
-      <c r="E8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
@@ -3116,61 +3845,117 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
+          <t>S2
+(09:00-11:00)</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>Trần Thị B</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="inlineStr"/>
+      <c r="D9" s="7" t="inlineStr"/>
+      <c r="E9" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="7" t="inlineStr"/>
+      <c r="H9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="10" t="n"/>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="inlineStr"/>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="G10" s="7" t="inlineStr"/>
+      <c r="H10" s="7" t="inlineStr"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
           <t>C2
 (15:00-17:00)</t>
         </is>
       </c>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>Phạm Văn D</t>
-        </is>
-      </c>
-      <c r="C9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
-      <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
-    </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>T2
-(19:30-21:30)</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
+      <c r="B11" s="7" t="inlineStr">
         <is>
           <t>Trần Thị B</t>
         </is>
       </c>
-      <c r="C10" s="7" t="inlineStr"/>
-      <c r="D10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: LAB01
-(Thực hành)</t>
-        </is>
-      </c>
-      <c r="E10" s="7" t="inlineStr"/>
-      <c r="F10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: LAB04
-(Thực hành)</t>
-        </is>
-      </c>
-      <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
+      <c r="C11" s="7" t="inlineStr"/>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+      <c r="G11" s="7" t="inlineStr"/>
+      <c r="H11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="n"/>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="inlineStr"/>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="F12" s="7" t="inlineStr"/>
+      <c r="G12" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+      <c r="H12" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3189,7 +3974,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3281,8 +4066,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C1
-(13:00-15:00)</t>
+          <t>S1
+(07:00-09:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -3290,16 +4075,16 @@
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C8" s="7" t="inlineStr"/>
+      <c r="C8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
       <c r="D8" s="7" t="inlineStr"/>
-      <c r="E8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
@@ -3307,61 +4092,117 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
+          <t>S2
+(09:00-11:00)</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>Trần Thị B</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="inlineStr"/>
+      <c r="D9" s="7" t="inlineStr"/>
+      <c r="E9" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="7" t="inlineStr"/>
+      <c r="H9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="10" t="n"/>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="inlineStr"/>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="G10" s="7" t="inlineStr"/>
+      <c r="H10" s="7" t="inlineStr"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
           <t>C2
 (15:00-17:00)</t>
         </is>
       </c>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>Phạm Văn D</t>
-        </is>
-      </c>
-      <c r="C9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
-      <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
-    </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>T2
-(19:30-21:30)</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
+      <c r="B11" s="7" t="inlineStr">
         <is>
           <t>Trần Thị B</t>
         </is>
       </c>
-      <c r="C10" s="7" t="inlineStr"/>
-      <c r="D10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: LAB01
-(Thực hành)</t>
-        </is>
-      </c>
-      <c r="E10" s="7" t="inlineStr"/>
-      <c r="F10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: LAB04
-(Thực hành)</t>
-        </is>
-      </c>
-      <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
+      <c r="C11" s="7" t="inlineStr"/>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+      <c r="G11" s="7" t="inlineStr"/>
+      <c r="H11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="n"/>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="inlineStr"/>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="F12" s="7" t="inlineStr"/>
+      <c r="G12" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
+        </is>
+      </c>
+      <c r="H12" s="9" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Cải thiện thuận toán GA
</commit_message>
<xml_diff>
--- a/timetabling_GA/results/HK1_CT02/TKB_HocKy_GiangVien.xlsx
+++ b/timetabling_GA/results/HK1_CT02/TKB_HocKy_GiangVien.xlsx
@@ -147,10 +147,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -516,7 +516,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -608,8 +608,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>S1
-(07:00-09:00)</t>
+          <t>C1
+(13:00-15:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -617,25 +617,25 @@
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Thiết kế Web
-Phòng: LAB01
-(Thực hành)</t>
-        </is>
-      </c>
+      <c r="C8" s="7" t="inlineStr"/>
       <c r="D8" s="7" t="inlineStr"/>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
+      <c r="H8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: LAB03
+(Thực hành)</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>S2
-(09:00-11:00)</t>
+          <t>C2
+(15:00-17:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -645,27 +645,20 @@
       </c>
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E9" s="7" t="inlineStr"/>
       <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Mạng máy tính
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
 Phòng: LAB01
 (Thực hành)</t>
         </is>
       </c>
+      <c r="H9" s="7" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" s="10" t="n"/>
+      <c r="A10" s="9" t="n"/>
       <c r="B10" s="7" t="inlineStr">
         <is>
           <t>Phạm Văn D</t>
@@ -674,22 +667,22 @@
       <c r="C10" s="7" t="inlineStr"/>
       <c r="D10" s="7" t="inlineStr"/>
       <c r="E10" s="7" t="inlineStr"/>
-      <c r="F10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="F10" s="7" t="inlineStr"/>
       <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
+      <c r="H10" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: R104
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="60" customHeight="1">
       <c r="A11" s="6" t="inlineStr">
         <is>
-          <t>C2
-(15:00-17:00)</t>
+          <t>T1
+(17:30-19:30)</t>
         </is>
       </c>
       <c r="B11" s="7" t="inlineStr">
@@ -700,36 +693,66 @@
       <c r="C11" s="7" t="inlineStr"/>
       <c r="D11" s="7" t="inlineStr"/>
       <c r="E11" s="7" t="inlineStr"/>
-      <c r="F11" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: LAB01
-(Thực hành)</t>
+      <c r="F11" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: R104
+(Lý thuyết)</t>
         </is>
       </c>
       <c r="G11" s="7" t="inlineStr"/>
       <c r="H11" s="7" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" s="10" t="n"/>
+      <c r="A12" s="9" t="n"/>
       <c r="B12" s="7" t="inlineStr">
         <is>
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C12" s="7" t="inlineStr"/>
+      <c r="C12" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: R101
+(Lý thuyết)</t>
+        </is>
+      </c>
       <c r="D12" s="7" t="inlineStr"/>
-      <c r="E12" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Mạng máy tính
-Phòng: R102
-(Lý thuyết)</t>
+      <c r="E12" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
         </is>
       </c>
       <c r="F12" s="7" t="inlineStr"/>
-      <c r="G12" s="8" t="inlineStr">
+      <c r="G12" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13" ht="60" customHeight="1">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>T2
+(19:30-21:30)</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="inlineStr"/>
+      <c r="D13" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL03
 Môn: Mạng máy tính
@@ -737,14 +760,10 @@
 (Thực hành)</t>
         </is>
       </c>
-      <c r="H12" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: R102
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E13" s="7" t="inlineStr"/>
+      <c r="F13" s="7" t="inlineStr"/>
+      <c r="G13" s="7" t="inlineStr"/>
+      <c r="H13" s="7" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -763,7 +782,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -855,8 +874,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>S1
-(07:00-09:00)</t>
+          <t>C1
+(13:00-15:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -864,25 +883,25 @@
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Thiết kế Web
-Phòng: LAB01
-(Thực hành)</t>
-        </is>
-      </c>
+      <c r="C8" s="7" t="inlineStr"/>
       <c r="D8" s="7" t="inlineStr"/>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
+      <c r="H8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: LAB03
+(Thực hành)</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>S2
-(09:00-11:00)</t>
+          <t>C2
+(15:00-17:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -892,27 +911,20 @@
       </c>
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E9" s="7" t="inlineStr"/>
       <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Mạng máy tính
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
 Phòng: LAB01
 (Thực hành)</t>
         </is>
       </c>
+      <c r="H9" s="7" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" s="10" t="n"/>
+      <c r="A10" s="9" t="n"/>
       <c r="B10" s="7" t="inlineStr">
         <is>
           <t>Phạm Văn D</t>
@@ -921,22 +933,22 @@
       <c r="C10" s="7" t="inlineStr"/>
       <c r="D10" s="7" t="inlineStr"/>
       <c r="E10" s="7" t="inlineStr"/>
-      <c r="F10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="F10" s="7" t="inlineStr"/>
       <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
+      <c r="H10" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: R104
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="60" customHeight="1">
       <c r="A11" s="6" t="inlineStr">
         <is>
-          <t>C2
-(15:00-17:00)</t>
+          <t>T1
+(17:30-19:30)</t>
         </is>
       </c>
       <c r="B11" s="7" t="inlineStr">
@@ -947,36 +959,66 @@
       <c r="C11" s="7" t="inlineStr"/>
       <c r="D11" s="7" t="inlineStr"/>
       <c r="E11" s="7" t="inlineStr"/>
-      <c r="F11" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: LAB01
-(Thực hành)</t>
+      <c r="F11" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: R104
+(Lý thuyết)</t>
         </is>
       </c>
       <c r="G11" s="7" t="inlineStr"/>
       <c r="H11" s="7" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" s="10" t="n"/>
+      <c r="A12" s="9" t="n"/>
       <c r="B12" s="7" t="inlineStr">
         <is>
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C12" s="7" t="inlineStr"/>
+      <c r="C12" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: R101
+(Lý thuyết)</t>
+        </is>
+      </c>
       <c r="D12" s="7" t="inlineStr"/>
-      <c r="E12" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Mạng máy tính
-Phòng: R102
-(Lý thuyết)</t>
+      <c r="E12" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
         </is>
       </c>
       <c r="F12" s="7" t="inlineStr"/>
-      <c r="G12" s="8" t="inlineStr">
+      <c r="G12" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13" ht="60" customHeight="1">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>T2
+(19:30-21:30)</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="inlineStr"/>
+      <c r="D13" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL03
 Môn: Mạng máy tính
@@ -984,14 +1026,10 @@
 (Thực hành)</t>
         </is>
       </c>
-      <c r="H12" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: R102
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E13" s="7" t="inlineStr"/>
+      <c r="F13" s="7" t="inlineStr"/>
+      <c r="G13" s="7" t="inlineStr"/>
+      <c r="H13" s="7" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1010,7 +1048,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1102,8 +1140,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>S1
-(07:00-09:00)</t>
+          <t>C1
+(13:00-15:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -1111,25 +1149,25 @@
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Thiết kế Web
-Phòng: LAB01
-(Thực hành)</t>
-        </is>
-      </c>
+      <c r="C8" s="7" t="inlineStr"/>
       <c r="D8" s="7" t="inlineStr"/>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
+      <c r="H8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: LAB03
+(Thực hành)</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>S2
-(09:00-11:00)</t>
+          <t>C2
+(15:00-17:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -1139,27 +1177,20 @@
       </c>
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E9" s="7" t="inlineStr"/>
       <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Mạng máy tính
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
 Phòng: LAB01
 (Thực hành)</t>
         </is>
       </c>
+      <c r="H9" s="7" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" s="10" t="n"/>
+      <c r="A10" s="9" t="n"/>
       <c r="B10" s="7" t="inlineStr">
         <is>
           <t>Phạm Văn D</t>
@@ -1168,22 +1199,22 @@
       <c r="C10" s="7" t="inlineStr"/>
       <c r="D10" s="7" t="inlineStr"/>
       <c r="E10" s="7" t="inlineStr"/>
-      <c r="F10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="F10" s="7" t="inlineStr"/>
       <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
+      <c r="H10" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: R104
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="60" customHeight="1">
       <c r="A11" s="6" t="inlineStr">
         <is>
-          <t>C2
-(15:00-17:00)</t>
+          <t>T1
+(17:30-19:30)</t>
         </is>
       </c>
       <c r="B11" s="7" t="inlineStr">
@@ -1194,36 +1225,66 @@
       <c r="C11" s="7" t="inlineStr"/>
       <c r="D11" s="7" t="inlineStr"/>
       <c r="E11" s="7" t="inlineStr"/>
-      <c r="F11" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: LAB01
-(Thực hành)</t>
+      <c r="F11" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: R104
+(Lý thuyết)</t>
         </is>
       </c>
       <c r="G11" s="7" t="inlineStr"/>
       <c r="H11" s="7" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" s="10" t="n"/>
+      <c r="A12" s="9" t="n"/>
       <c r="B12" s="7" t="inlineStr">
         <is>
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C12" s="7" t="inlineStr"/>
+      <c r="C12" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: R101
+(Lý thuyết)</t>
+        </is>
+      </c>
       <c r="D12" s="7" t="inlineStr"/>
-      <c r="E12" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Mạng máy tính
-Phòng: R102
-(Lý thuyết)</t>
+      <c r="E12" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
         </is>
       </c>
       <c r="F12" s="7" t="inlineStr"/>
-      <c r="G12" s="8" t="inlineStr">
+      <c r="G12" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13" ht="60" customHeight="1">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>T2
+(19:30-21:30)</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="inlineStr"/>
+      <c r="D13" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL03
 Môn: Mạng máy tính
@@ -1231,14 +1292,10 @@
 (Thực hành)</t>
         </is>
       </c>
-      <c r="H12" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: R102
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E13" s="7" t="inlineStr"/>
+      <c r="F13" s="7" t="inlineStr"/>
+      <c r="G13" s="7" t="inlineStr"/>
+      <c r="H13" s="7" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1257,7 +1314,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1349,8 +1406,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>S1
-(07:00-09:00)</t>
+          <t>C1
+(13:00-15:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -1358,25 +1415,25 @@
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Thiết kế Web
-Phòng: LAB01
-(Thực hành)</t>
-        </is>
-      </c>
+      <c r="C8" s="7" t="inlineStr"/>
       <c r="D8" s="7" t="inlineStr"/>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
+      <c r="H8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: LAB03
+(Thực hành)</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>S2
-(09:00-11:00)</t>
+          <t>C2
+(15:00-17:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -1386,27 +1443,20 @@
       </c>
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E9" s="7" t="inlineStr"/>
       <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Mạng máy tính
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
 Phòng: LAB01
 (Thực hành)</t>
         </is>
       </c>
+      <c r="H9" s="7" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" s="10" t="n"/>
+      <c r="A10" s="9" t="n"/>
       <c r="B10" s="7" t="inlineStr">
         <is>
           <t>Phạm Văn D</t>
@@ -1415,22 +1465,22 @@
       <c r="C10" s="7" t="inlineStr"/>
       <c r="D10" s="7" t="inlineStr"/>
       <c r="E10" s="7" t="inlineStr"/>
-      <c r="F10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="F10" s="7" t="inlineStr"/>
       <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
+      <c r="H10" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: R104
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="60" customHeight="1">
       <c r="A11" s="6" t="inlineStr">
         <is>
-          <t>C2
-(15:00-17:00)</t>
+          <t>T1
+(17:30-19:30)</t>
         </is>
       </c>
       <c r="B11" s="7" t="inlineStr">
@@ -1441,36 +1491,66 @@
       <c r="C11" s="7" t="inlineStr"/>
       <c r="D11" s="7" t="inlineStr"/>
       <c r="E11" s="7" t="inlineStr"/>
-      <c r="F11" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: LAB01
-(Thực hành)</t>
+      <c r="F11" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: R104
+(Lý thuyết)</t>
         </is>
       </c>
       <c r="G11" s="7" t="inlineStr"/>
       <c r="H11" s="7" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" s="10" t="n"/>
+      <c r="A12" s="9" t="n"/>
       <c r="B12" s="7" t="inlineStr">
         <is>
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C12" s="7" t="inlineStr"/>
+      <c r="C12" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: R101
+(Lý thuyết)</t>
+        </is>
+      </c>
       <c r="D12" s="7" t="inlineStr"/>
-      <c r="E12" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Mạng máy tính
-Phòng: R102
-(Lý thuyết)</t>
+      <c r="E12" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
         </is>
       </c>
       <c r="F12" s="7" t="inlineStr"/>
-      <c r="G12" s="8" t="inlineStr">
+      <c r="G12" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13" ht="60" customHeight="1">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>T2
+(19:30-21:30)</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="inlineStr"/>
+      <c r="D13" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL03
 Môn: Mạng máy tính
@@ -1478,14 +1558,10 @@
 (Thực hành)</t>
         </is>
       </c>
-      <c r="H12" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: R102
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E13" s="7" t="inlineStr"/>
+      <c r="F13" s="7" t="inlineStr"/>
+      <c r="G13" s="7" t="inlineStr"/>
+      <c r="H13" s="7" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1504,7 +1580,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1596,8 +1672,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>S1
-(07:00-09:00)</t>
+          <t>C1
+(13:00-15:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -1605,25 +1681,25 @@
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Thiết kế Web
-Phòng: LAB01
-(Thực hành)</t>
-        </is>
-      </c>
+      <c r="C8" s="7" t="inlineStr"/>
       <c r="D8" s="7" t="inlineStr"/>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
+      <c r="H8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: LAB03
+(Thực hành)</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>S2
-(09:00-11:00)</t>
+          <t>C2
+(15:00-17:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -1633,27 +1709,20 @@
       </c>
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E9" s="7" t="inlineStr"/>
       <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Mạng máy tính
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
 Phòng: LAB01
 (Thực hành)</t>
         </is>
       </c>
+      <c r="H9" s="7" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" s="10" t="n"/>
+      <c r="A10" s="9" t="n"/>
       <c r="B10" s="7" t="inlineStr">
         <is>
           <t>Phạm Văn D</t>
@@ -1662,22 +1731,22 @@
       <c r="C10" s="7" t="inlineStr"/>
       <c r="D10" s="7" t="inlineStr"/>
       <c r="E10" s="7" t="inlineStr"/>
-      <c r="F10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="F10" s="7" t="inlineStr"/>
       <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
+      <c r="H10" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: R104
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="60" customHeight="1">
       <c r="A11" s="6" t="inlineStr">
         <is>
-          <t>C2
-(15:00-17:00)</t>
+          <t>T1
+(17:30-19:30)</t>
         </is>
       </c>
       <c r="B11" s="7" t="inlineStr">
@@ -1688,36 +1757,66 @@
       <c r="C11" s="7" t="inlineStr"/>
       <c r="D11" s="7" t="inlineStr"/>
       <c r="E11" s="7" t="inlineStr"/>
-      <c r="F11" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: LAB01
-(Thực hành)</t>
+      <c r="F11" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: R104
+(Lý thuyết)</t>
         </is>
       </c>
       <c r="G11" s="7" t="inlineStr"/>
       <c r="H11" s="7" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" s="10" t="n"/>
+      <c r="A12" s="9" t="n"/>
       <c r="B12" s="7" t="inlineStr">
         <is>
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C12" s="7" t="inlineStr"/>
+      <c r="C12" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: R101
+(Lý thuyết)</t>
+        </is>
+      </c>
       <c r="D12" s="7" t="inlineStr"/>
-      <c r="E12" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Mạng máy tính
-Phòng: R102
-(Lý thuyết)</t>
+      <c r="E12" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
         </is>
       </c>
       <c r="F12" s="7" t="inlineStr"/>
-      <c r="G12" s="8" t="inlineStr">
+      <c r="G12" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13" ht="60" customHeight="1">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>T2
+(19:30-21:30)</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="inlineStr"/>
+      <c r="D13" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL03
 Môn: Mạng máy tính
@@ -1725,14 +1824,10 @@
 (Thực hành)</t>
         </is>
       </c>
-      <c r="H12" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: R102
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E13" s="7" t="inlineStr"/>
+      <c r="F13" s="7" t="inlineStr"/>
+      <c r="G13" s="7" t="inlineStr"/>
+      <c r="H13" s="7" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1751,7 +1846,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1843,8 +1938,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>S1
-(07:00-09:00)</t>
+          <t>C1
+(13:00-15:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -1852,25 +1947,25 @@
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Thiết kế Web
-Phòng: LAB01
-(Thực hành)</t>
-        </is>
-      </c>
+      <c r="C8" s="7" t="inlineStr"/>
       <c r="D8" s="7" t="inlineStr"/>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
+      <c r="H8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: LAB03
+(Thực hành)</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>S2
-(09:00-11:00)</t>
+          <t>C2
+(15:00-17:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -1880,27 +1975,20 @@
       </c>
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E9" s="7" t="inlineStr"/>
       <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Mạng máy tính
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
 Phòng: LAB01
 (Thực hành)</t>
         </is>
       </c>
+      <c r="H9" s="7" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" s="10" t="n"/>
+      <c r="A10" s="9" t="n"/>
       <c r="B10" s="7" t="inlineStr">
         <is>
           <t>Phạm Văn D</t>
@@ -1909,22 +1997,22 @@
       <c r="C10" s="7" t="inlineStr"/>
       <c r="D10" s="7" t="inlineStr"/>
       <c r="E10" s="7" t="inlineStr"/>
-      <c r="F10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="F10" s="7" t="inlineStr"/>
       <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
+      <c r="H10" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: R104
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="60" customHeight="1">
       <c r="A11" s="6" t="inlineStr">
         <is>
-          <t>C2
-(15:00-17:00)</t>
+          <t>T1
+(17:30-19:30)</t>
         </is>
       </c>
       <c r="B11" s="7" t="inlineStr">
@@ -1935,36 +2023,66 @@
       <c r="C11" s="7" t="inlineStr"/>
       <c r="D11" s="7" t="inlineStr"/>
       <c r="E11" s="7" t="inlineStr"/>
-      <c r="F11" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: LAB01
-(Thực hành)</t>
+      <c r="F11" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: R104
+(Lý thuyết)</t>
         </is>
       </c>
       <c r="G11" s="7" t="inlineStr"/>
       <c r="H11" s="7" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" s="10" t="n"/>
+      <c r="A12" s="9" t="n"/>
       <c r="B12" s="7" t="inlineStr">
         <is>
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C12" s="7" t="inlineStr"/>
+      <c r="C12" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: R101
+(Lý thuyết)</t>
+        </is>
+      </c>
       <c r="D12" s="7" t="inlineStr"/>
-      <c r="E12" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Mạng máy tính
-Phòng: R102
-(Lý thuyết)</t>
+      <c r="E12" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
         </is>
       </c>
       <c r="F12" s="7" t="inlineStr"/>
-      <c r="G12" s="8" t="inlineStr">
+      <c r="G12" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13" ht="60" customHeight="1">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>T2
+(19:30-21:30)</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="inlineStr"/>
+      <c r="D13" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL03
 Môn: Mạng máy tính
@@ -1972,14 +2090,10 @@
 (Thực hành)</t>
         </is>
       </c>
-      <c r="H12" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: R102
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E13" s="7" t="inlineStr"/>
+      <c r="F13" s="7" t="inlineStr"/>
+      <c r="G13" s="7" t="inlineStr"/>
+      <c r="H13" s="7" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1998,7 +2112,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2090,8 +2204,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>S1
-(07:00-09:00)</t>
+          <t>C1
+(13:00-15:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -2099,25 +2213,25 @@
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Thiết kế Web
-Phòng: LAB01
-(Thực hành)</t>
-        </is>
-      </c>
+      <c r="C8" s="7" t="inlineStr"/>
       <c r="D8" s="7" t="inlineStr"/>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
+      <c r="H8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: LAB03
+(Thực hành)</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>S2
-(09:00-11:00)</t>
+          <t>C2
+(15:00-17:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -2127,27 +2241,20 @@
       </c>
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E9" s="7" t="inlineStr"/>
       <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Mạng máy tính
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
 Phòng: LAB01
 (Thực hành)</t>
         </is>
       </c>
+      <c r="H9" s="7" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" s="10" t="n"/>
+      <c r="A10" s="9" t="n"/>
       <c r="B10" s="7" t="inlineStr">
         <is>
           <t>Phạm Văn D</t>
@@ -2156,22 +2263,22 @@
       <c r="C10" s="7" t="inlineStr"/>
       <c r="D10" s="7" t="inlineStr"/>
       <c r="E10" s="7" t="inlineStr"/>
-      <c r="F10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="F10" s="7" t="inlineStr"/>
       <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
+      <c r="H10" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: R104
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="60" customHeight="1">
       <c r="A11" s="6" t="inlineStr">
         <is>
-          <t>C2
-(15:00-17:00)</t>
+          <t>T1
+(17:30-19:30)</t>
         </is>
       </c>
       <c r="B11" s="7" t="inlineStr">
@@ -2182,36 +2289,66 @@
       <c r="C11" s="7" t="inlineStr"/>
       <c r="D11" s="7" t="inlineStr"/>
       <c r="E11" s="7" t="inlineStr"/>
-      <c r="F11" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: LAB01
-(Thực hành)</t>
+      <c r="F11" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: R104
+(Lý thuyết)</t>
         </is>
       </c>
       <c r="G11" s="7" t="inlineStr"/>
       <c r="H11" s="7" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" s="10" t="n"/>
+      <c r="A12" s="9" t="n"/>
       <c r="B12" s="7" t="inlineStr">
         <is>
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C12" s="7" t="inlineStr"/>
+      <c r="C12" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: R101
+(Lý thuyết)</t>
+        </is>
+      </c>
       <c r="D12" s="7" t="inlineStr"/>
-      <c r="E12" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Mạng máy tính
-Phòng: R102
-(Lý thuyết)</t>
+      <c r="E12" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
         </is>
       </c>
       <c r="F12" s="7" t="inlineStr"/>
-      <c r="G12" s="8" t="inlineStr">
+      <c r="G12" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13" ht="60" customHeight="1">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>T2
+(19:30-21:30)</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="inlineStr"/>
+      <c r="D13" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL03
 Môn: Mạng máy tính
@@ -2219,14 +2356,10 @@
 (Thực hành)</t>
         </is>
       </c>
-      <c r="H12" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: R102
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E13" s="7" t="inlineStr"/>
+      <c r="F13" s="7" t="inlineStr"/>
+      <c r="G13" s="7" t="inlineStr"/>
+      <c r="H13" s="7" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2245,7 +2378,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2337,8 +2470,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>S1
-(07:00-09:00)</t>
+          <t>C1
+(13:00-15:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -2346,25 +2479,25 @@
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Thiết kế Web
-Phòng: LAB01
-(Thực hành)</t>
-        </is>
-      </c>
+      <c r="C8" s="7" t="inlineStr"/>
       <c r="D8" s="7" t="inlineStr"/>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
+      <c r="H8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: LAB03
+(Thực hành)</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>S2
-(09:00-11:00)</t>
+          <t>C2
+(15:00-17:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -2374,27 +2507,20 @@
       </c>
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E9" s="7" t="inlineStr"/>
       <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Mạng máy tính
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
 Phòng: LAB01
 (Thực hành)</t>
         </is>
       </c>
+      <c r="H9" s="7" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" s="10" t="n"/>
+      <c r="A10" s="9" t="n"/>
       <c r="B10" s="7" t="inlineStr">
         <is>
           <t>Phạm Văn D</t>
@@ -2403,22 +2529,22 @@
       <c r="C10" s="7" t="inlineStr"/>
       <c r="D10" s="7" t="inlineStr"/>
       <c r="E10" s="7" t="inlineStr"/>
-      <c r="F10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="F10" s="7" t="inlineStr"/>
       <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
+      <c r="H10" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: R104
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="60" customHeight="1">
       <c r="A11" s="6" t="inlineStr">
         <is>
-          <t>C2
-(15:00-17:00)</t>
+          <t>T1
+(17:30-19:30)</t>
         </is>
       </c>
       <c r="B11" s="7" t="inlineStr">
@@ -2429,36 +2555,66 @@
       <c r="C11" s="7" t="inlineStr"/>
       <c r="D11" s="7" t="inlineStr"/>
       <c r="E11" s="7" t="inlineStr"/>
-      <c r="F11" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: LAB01
-(Thực hành)</t>
+      <c r="F11" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: R104
+(Lý thuyết)</t>
         </is>
       </c>
       <c r="G11" s="7" t="inlineStr"/>
       <c r="H11" s="7" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" s="10" t="n"/>
+      <c r="A12" s="9" t="n"/>
       <c r="B12" s="7" t="inlineStr">
         <is>
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C12" s="7" t="inlineStr"/>
+      <c r="C12" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: R101
+(Lý thuyết)</t>
+        </is>
+      </c>
       <c r="D12" s="7" t="inlineStr"/>
-      <c r="E12" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Mạng máy tính
-Phòng: R102
-(Lý thuyết)</t>
+      <c r="E12" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
         </is>
       </c>
       <c r="F12" s="7" t="inlineStr"/>
-      <c r="G12" s="8" t="inlineStr">
+      <c r="G12" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13" ht="60" customHeight="1">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>T2
+(19:30-21:30)</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="inlineStr"/>
+      <c r="D13" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL03
 Môn: Mạng máy tính
@@ -2466,14 +2622,10 @@
 (Thực hành)</t>
         </is>
       </c>
-      <c r="H12" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: R102
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E13" s="7" t="inlineStr"/>
+      <c r="F13" s="7" t="inlineStr"/>
+      <c r="G13" s="7" t="inlineStr"/>
+      <c r="H13" s="7" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2492,7 +2644,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2584,8 +2736,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>S1
-(07:00-09:00)</t>
+          <t>C1
+(13:00-15:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -2593,25 +2745,25 @@
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Thiết kế Web
-Phòng: LAB01
-(Thực hành)</t>
-        </is>
-      </c>
+      <c r="C8" s="7" t="inlineStr"/>
       <c r="D8" s="7" t="inlineStr"/>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
+      <c r="H8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: LAB03
+(Thực hành)</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>S2
-(09:00-11:00)</t>
+          <t>C2
+(15:00-17:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -2621,27 +2773,20 @@
       </c>
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E9" s="7" t="inlineStr"/>
       <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Mạng máy tính
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
 Phòng: LAB01
 (Thực hành)</t>
         </is>
       </c>
+      <c r="H9" s="7" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" s="10" t="n"/>
+      <c r="A10" s="9" t="n"/>
       <c r="B10" s="7" t="inlineStr">
         <is>
           <t>Phạm Văn D</t>
@@ -2650,22 +2795,22 @@
       <c r="C10" s="7" t="inlineStr"/>
       <c r="D10" s="7" t="inlineStr"/>
       <c r="E10" s="7" t="inlineStr"/>
-      <c r="F10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="F10" s="7" t="inlineStr"/>
       <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
+      <c r="H10" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: R104
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="60" customHeight="1">
       <c r="A11" s="6" t="inlineStr">
         <is>
-          <t>C2
-(15:00-17:00)</t>
+          <t>T1
+(17:30-19:30)</t>
         </is>
       </c>
       <c r="B11" s="7" t="inlineStr">
@@ -2676,36 +2821,66 @@
       <c r="C11" s="7" t="inlineStr"/>
       <c r="D11" s="7" t="inlineStr"/>
       <c r="E11" s="7" t="inlineStr"/>
-      <c r="F11" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: LAB01
-(Thực hành)</t>
+      <c r="F11" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: R104
+(Lý thuyết)</t>
         </is>
       </c>
       <c r="G11" s="7" t="inlineStr"/>
       <c r="H11" s="7" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" s="10" t="n"/>
+      <c r="A12" s="9" t="n"/>
       <c r="B12" s="7" t="inlineStr">
         <is>
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C12" s="7" t="inlineStr"/>
+      <c r="C12" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: R101
+(Lý thuyết)</t>
+        </is>
+      </c>
       <c r="D12" s="7" t="inlineStr"/>
-      <c r="E12" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Mạng máy tính
-Phòng: R102
-(Lý thuyết)</t>
+      <c r="E12" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
         </is>
       </c>
       <c r="F12" s="7" t="inlineStr"/>
-      <c r="G12" s="8" t="inlineStr">
+      <c r="G12" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13" ht="60" customHeight="1">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>T2
+(19:30-21:30)</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="inlineStr"/>
+      <c r="D13" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL03
 Môn: Mạng máy tính
@@ -2713,14 +2888,10 @@
 (Thực hành)</t>
         </is>
       </c>
-      <c r="H12" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: R102
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E13" s="7" t="inlineStr"/>
+      <c r="F13" s="7" t="inlineStr"/>
+      <c r="G13" s="7" t="inlineStr"/>
+      <c r="H13" s="7" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2739,7 +2910,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2831,8 +3002,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>S1
-(07:00-09:00)</t>
+          <t>C1
+(13:00-15:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -2840,25 +3011,25 @@
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Thiết kế Web
-Phòng: LAB01
-(Thực hành)</t>
-        </is>
-      </c>
+      <c r="C8" s="7" t="inlineStr"/>
       <c r="D8" s="7" t="inlineStr"/>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
+      <c r="H8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: LAB03
+(Thực hành)</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>S2
-(09:00-11:00)</t>
+          <t>C2
+(15:00-17:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -2868,27 +3039,20 @@
       </c>
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E9" s="7" t="inlineStr"/>
       <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Mạng máy tính
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
 Phòng: LAB01
 (Thực hành)</t>
         </is>
       </c>
+      <c r="H9" s="7" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" s="10" t="n"/>
+      <c r="A10" s="9" t="n"/>
       <c r="B10" s="7" t="inlineStr">
         <is>
           <t>Phạm Văn D</t>
@@ -2897,22 +3061,22 @@
       <c r="C10" s="7" t="inlineStr"/>
       <c r="D10" s="7" t="inlineStr"/>
       <c r="E10" s="7" t="inlineStr"/>
-      <c r="F10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="F10" s="7" t="inlineStr"/>
       <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
+      <c r="H10" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: R104
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="60" customHeight="1">
       <c r="A11" s="6" t="inlineStr">
         <is>
-          <t>C2
-(15:00-17:00)</t>
+          <t>T1
+(17:30-19:30)</t>
         </is>
       </c>
       <c r="B11" s="7" t="inlineStr">
@@ -2923,36 +3087,66 @@
       <c r="C11" s="7" t="inlineStr"/>
       <c r="D11" s="7" t="inlineStr"/>
       <c r="E11" s="7" t="inlineStr"/>
-      <c r="F11" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: LAB01
-(Thực hành)</t>
+      <c r="F11" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: R104
+(Lý thuyết)</t>
         </is>
       </c>
       <c r="G11" s="7" t="inlineStr"/>
       <c r="H11" s="7" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" s="10" t="n"/>
+      <c r="A12" s="9" t="n"/>
       <c r="B12" s="7" t="inlineStr">
         <is>
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C12" s="7" t="inlineStr"/>
+      <c r="C12" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: R101
+(Lý thuyết)</t>
+        </is>
+      </c>
       <c r="D12" s="7" t="inlineStr"/>
-      <c r="E12" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Mạng máy tính
-Phòng: R102
-(Lý thuyết)</t>
+      <c r="E12" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
         </is>
       </c>
       <c r="F12" s="7" t="inlineStr"/>
-      <c r="G12" s="8" t="inlineStr">
+      <c r="G12" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13" ht="60" customHeight="1">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>T2
+(19:30-21:30)</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="inlineStr"/>
+      <c r="D13" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL03
 Môn: Mạng máy tính
@@ -2960,14 +3154,10 @@
 (Thực hành)</t>
         </is>
       </c>
-      <c r="H12" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: R102
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E13" s="7" t="inlineStr"/>
+      <c r="F13" s="7" t="inlineStr"/>
+      <c r="G13" s="7" t="inlineStr"/>
+      <c r="H13" s="7" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2986,7 +3176,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3078,8 +3268,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>S1
-(07:00-09:00)</t>
+          <t>C1
+(13:00-15:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -3087,25 +3277,25 @@
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Thiết kế Web
-Phòng: LAB01
-(Thực hành)</t>
-        </is>
-      </c>
+      <c r="C8" s="7" t="inlineStr"/>
       <c r="D8" s="7" t="inlineStr"/>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
+      <c r="H8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: LAB03
+(Thực hành)</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>S2
-(09:00-11:00)</t>
+          <t>C2
+(15:00-17:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -3115,27 +3305,20 @@
       </c>
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E9" s="7" t="inlineStr"/>
       <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Mạng máy tính
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
 Phòng: LAB01
 (Thực hành)</t>
         </is>
       </c>
+      <c r="H9" s="7" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" s="10" t="n"/>
+      <c r="A10" s="9" t="n"/>
       <c r="B10" s="7" t="inlineStr">
         <is>
           <t>Phạm Văn D</t>
@@ -3144,22 +3327,22 @@
       <c r="C10" s="7" t="inlineStr"/>
       <c r="D10" s="7" t="inlineStr"/>
       <c r="E10" s="7" t="inlineStr"/>
-      <c r="F10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="F10" s="7" t="inlineStr"/>
       <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
+      <c r="H10" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: R104
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="60" customHeight="1">
       <c r="A11" s="6" t="inlineStr">
         <is>
-          <t>C2
-(15:00-17:00)</t>
+          <t>T1
+(17:30-19:30)</t>
         </is>
       </c>
       <c r="B11" s="7" t="inlineStr">
@@ -3170,36 +3353,66 @@
       <c r="C11" s="7" t="inlineStr"/>
       <c r="D11" s="7" t="inlineStr"/>
       <c r="E11" s="7" t="inlineStr"/>
-      <c r="F11" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: LAB01
-(Thực hành)</t>
+      <c r="F11" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: R104
+(Lý thuyết)</t>
         </is>
       </c>
       <c r="G11" s="7" t="inlineStr"/>
       <c r="H11" s="7" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" s="10" t="n"/>
+      <c r="A12" s="9" t="n"/>
       <c r="B12" s="7" t="inlineStr">
         <is>
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C12" s="7" t="inlineStr"/>
+      <c r="C12" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: R101
+(Lý thuyết)</t>
+        </is>
+      </c>
       <c r="D12" s="7" t="inlineStr"/>
-      <c r="E12" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Mạng máy tính
-Phòng: R102
-(Lý thuyết)</t>
+      <c r="E12" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
         </is>
       </c>
       <c r="F12" s="7" t="inlineStr"/>
-      <c r="G12" s="8" t="inlineStr">
+      <c r="G12" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13" ht="60" customHeight="1">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>T2
+(19:30-21:30)</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="inlineStr"/>
+      <c r="D13" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL03
 Môn: Mạng máy tính
@@ -3207,14 +3420,10 @@
 (Thực hành)</t>
         </is>
       </c>
-      <c r="H12" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: R102
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E13" s="7" t="inlineStr"/>
+      <c r="F13" s="7" t="inlineStr"/>
+      <c r="G13" s="7" t="inlineStr"/>
+      <c r="H13" s="7" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3233,7 +3442,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3325,8 +3534,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>S1
-(07:00-09:00)</t>
+          <t>C1
+(13:00-15:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -3334,25 +3543,25 @@
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Thiết kế Web
-Phòng: LAB01
-(Thực hành)</t>
-        </is>
-      </c>
+      <c r="C8" s="7" t="inlineStr"/>
       <c r="D8" s="7" t="inlineStr"/>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
+      <c r="H8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: LAB03
+(Thực hành)</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>S2
-(09:00-11:00)</t>
+          <t>C2
+(15:00-17:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -3362,27 +3571,20 @@
       </c>
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E9" s="7" t="inlineStr"/>
       <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Mạng máy tính
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
 Phòng: LAB01
 (Thực hành)</t>
         </is>
       </c>
+      <c r="H9" s="7" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" s="10" t="n"/>
+      <c r="A10" s="9" t="n"/>
       <c r="B10" s="7" t="inlineStr">
         <is>
           <t>Phạm Văn D</t>
@@ -3391,22 +3593,22 @@
       <c r="C10" s="7" t="inlineStr"/>
       <c r="D10" s="7" t="inlineStr"/>
       <c r="E10" s="7" t="inlineStr"/>
-      <c r="F10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="F10" s="7" t="inlineStr"/>
       <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
+      <c r="H10" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: R104
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="60" customHeight="1">
       <c r="A11" s="6" t="inlineStr">
         <is>
-          <t>C2
-(15:00-17:00)</t>
+          <t>T1
+(17:30-19:30)</t>
         </is>
       </c>
       <c r="B11" s="7" t="inlineStr">
@@ -3417,36 +3619,66 @@
       <c r="C11" s="7" t="inlineStr"/>
       <c r="D11" s="7" t="inlineStr"/>
       <c r="E11" s="7" t="inlineStr"/>
-      <c r="F11" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: LAB01
-(Thực hành)</t>
+      <c r="F11" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: R104
+(Lý thuyết)</t>
         </is>
       </c>
       <c r="G11" s="7" t="inlineStr"/>
       <c r="H11" s="7" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" s="10" t="n"/>
+      <c r="A12" s="9" t="n"/>
       <c r="B12" s="7" t="inlineStr">
         <is>
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C12" s="7" t="inlineStr"/>
+      <c r="C12" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: R101
+(Lý thuyết)</t>
+        </is>
+      </c>
       <c r="D12" s="7" t="inlineStr"/>
-      <c r="E12" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Mạng máy tính
-Phòng: R102
-(Lý thuyết)</t>
+      <c r="E12" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
         </is>
       </c>
       <c r="F12" s="7" t="inlineStr"/>
-      <c r="G12" s="8" t="inlineStr">
+      <c r="G12" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13" ht="60" customHeight="1">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>T2
+(19:30-21:30)</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="inlineStr"/>
+      <c r="D13" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL03
 Môn: Mạng máy tính
@@ -3454,14 +3686,10 @@
 (Thực hành)</t>
         </is>
       </c>
-      <c r="H12" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: R102
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E13" s="7" t="inlineStr"/>
+      <c r="F13" s="7" t="inlineStr"/>
+      <c r="G13" s="7" t="inlineStr"/>
+      <c r="H13" s="7" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3480,7 +3708,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3572,8 +3800,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>S1
-(07:00-09:00)</t>
+          <t>C1
+(13:00-15:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -3581,25 +3809,25 @@
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Thiết kế Web
-Phòng: LAB01
-(Thực hành)</t>
-        </is>
-      </c>
+      <c r="C8" s="7" t="inlineStr"/>
       <c r="D8" s="7" t="inlineStr"/>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
+      <c r="H8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: LAB03
+(Thực hành)</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>S2
-(09:00-11:00)</t>
+          <t>C2
+(15:00-17:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -3609,27 +3837,20 @@
       </c>
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E9" s="7" t="inlineStr"/>
       <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Mạng máy tính
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
 Phòng: LAB01
 (Thực hành)</t>
         </is>
       </c>
+      <c r="H9" s="7" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" s="10" t="n"/>
+      <c r="A10" s="9" t="n"/>
       <c r="B10" s="7" t="inlineStr">
         <is>
           <t>Phạm Văn D</t>
@@ -3638,22 +3859,22 @@
       <c r="C10" s="7" t="inlineStr"/>
       <c r="D10" s="7" t="inlineStr"/>
       <c r="E10" s="7" t="inlineStr"/>
-      <c r="F10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="F10" s="7" t="inlineStr"/>
       <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
+      <c r="H10" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: R104
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="60" customHeight="1">
       <c r="A11" s="6" t="inlineStr">
         <is>
-          <t>C2
-(15:00-17:00)</t>
+          <t>T1
+(17:30-19:30)</t>
         </is>
       </c>
       <c r="B11" s="7" t="inlineStr">
@@ -3664,36 +3885,66 @@
       <c r="C11" s="7" t="inlineStr"/>
       <c r="D11" s="7" t="inlineStr"/>
       <c r="E11" s="7" t="inlineStr"/>
-      <c r="F11" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: LAB01
-(Thực hành)</t>
+      <c r="F11" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: R104
+(Lý thuyết)</t>
         </is>
       </c>
       <c r="G11" s="7" t="inlineStr"/>
       <c r="H11" s="7" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" s="10" t="n"/>
+      <c r="A12" s="9" t="n"/>
       <c r="B12" s="7" t="inlineStr">
         <is>
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C12" s="7" t="inlineStr"/>
+      <c r="C12" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: R101
+(Lý thuyết)</t>
+        </is>
+      </c>
       <c r="D12" s="7" t="inlineStr"/>
-      <c r="E12" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Mạng máy tính
-Phòng: R102
-(Lý thuyết)</t>
+      <c r="E12" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
         </is>
       </c>
       <c r="F12" s="7" t="inlineStr"/>
-      <c r="G12" s="8" t="inlineStr">
+      <c r="G12" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13" ht="60" customHeight="1">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>T2
+(19:30-21:30)</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="inlineStr"/>
+      <c r="D13" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL03
 Môn: Mạng máy tính
@@ -3701,14 +3952,10 @@
 (Thực hành)</t>
         </is>
       </c>
-      <c r="H12" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: R102
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E13" s="7" t="inlineStr"/>
+      <c r="F13" s="7" t="inlineStr"/>
+      <c r="G13" s="7" t="inlineStr"/>
+      <c r="H13" s="7" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3727,7 +3974,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3819,8 +4066,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>S1
-(07:00-09:00)</t>
+          <t>C1
+(13:00-15:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -3828,25 +4075,25 @@
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Thiết kế Web
-Phòng: LAB01
-(Thực hành)</t>
-        </is>
-      </c>
+      <c r="C8" s="7" t="inlineStr"/>
       <c r="D8" s="7" t="inlineStr"/>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
+      <c r="H8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: LAB03
+(Thực hành)</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>S2
-(09:00-11:00)</t>
+          <t>C2
+(15:00-17:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -3856,27 +4103,20 @@
       </c>
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E9" s="7" t="inlineStr"/>
       <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Mạng máy tính
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
 Phòng: LAB01
 (Thực hành)</t>
         </is>
       </c>
+      <c r="H9" s="7" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" s="10" t="n"/>
+      <c r="A10" s="9" t="n"/>
       <c r="B10" s="7" t="inlineStr">
         <is>
           <t>Phạm Văn D</t>
@@ -3885,22 +4125,22 @@
       <c r="C10" s="7" t="inlineStr"/>
       <c r="D10" s="7" t="inlineStr"/>
       <c r="E10" s="7" t="inlineStr"/>
-      <c r="F10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="F10" s="7" t="inlineStr"/>
       <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
+      <c r="H10" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: R104
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="60" customHeight="1">
       <c r="A11" s="6" t="inlineStr">
         <is>
-          <t>C2
-(15:00-17:00)</t>
+          <t>T1
+(17:30-19:30)</t>
         </is>
       </c>
       <c r="B11" s="7" t="inlineStr">
@@ -3911,36 +4151,66 @@
       <c r="C11" s="7" t="inlineStr"/>
       <c r="D11" s="7" t="inlineStr"/>
       <c r="E11" s="7" t="inlineStr"/>
-      <c r="F11" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: LAB01
-(Thực hành)</t>
+      <c r="F11" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: R104
+(Lý thuyết)</t>
         </is>
       </c>
       <c r="G11" s="7" t="inlineStr"/>
       <c r="H11" s="7" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" s="10" t="n"/>
+      <c r="A12" s="9" t="n"/>
       <c r="B12" s="7" t="inlineStr">
         <is>
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C12" s="7" t="inlineStr"/>
+      <c r="C12" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: R101
+(Lý thuyết)</t>
+        </is>
+      </c>
       <c r="D12" s="7" t="inlineStr"/>
-      <c r="E12" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Mạng máy tính
-Phòng: R102
-(Lý thuyết)</t>
+      <c r="E12" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
         </is>
       </c>
       <c r="F12" s="7" t="inlineStr"/>
-      <c r="G12" s="8" t="inlineStr">
+      <c r="G12" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13" ht="60" customHeight="1">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>T2
+(19:30-21:30)</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="inlineStr"/>
+      <c r="D13" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL03
 Môn: Mạng máy tính
@@ -3948,14 +4218,10 @@
 (Thực hành)</t>
         </is>
       </c>
-      <c r="H12" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: R102
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E13" s="7" t="inlineStr"/>
+      <c r="F13" s="7" t="inlineStr"/>
+      <c r="G13" s="7" t="inlineStr"/>
+      <c r="H13" s="7" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3974,7 +4240,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4066,8 +4332,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>S1
-(07:00-09:00)</t>
+          <t>C1
+(13:00-15:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -4075,25 +4341,25 @@
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Thiết kế Web
-Phòng: LAB01
-(Thực hành)</t>
-        </is>
-      </c>
+      <c r="C8" s="7" t="inlineStr"/>
       <c r="D8" s="7" t="inlineStr"/>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
+      <c r="H8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: LAB03
+(Thực hành)</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>S2
-(09:00-11:00)</t>
+          <t>C2
+(15:00-17:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -4103,27 +4369,20 @@
       </c>
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E9" s="7" t="inlineStr"/>
       <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Mạng máy tính
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
 Phòng: LAB01
 (Thực hành)</t>
         </is>
       </c>
+      <c r="H9" s="7" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" s="10" t="n"/>
+      <c r="A10" s="9" t="n"/>
       <c r="B10" s="7" t="inlineStr">
         <is>
           <t>Phạm Văn D</t>
@@ -4132,22 +4391,22 @@
       <c r="C10" s="7" t="inlineStr"/>
       <c r="D10" s="7" t="inlineStr"/>
       <c r="E10" s="7" t="inlineStr"/>
-      <c r="F10" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Thiết kế Web
-Phòng: R103
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="F10" s="7" t="inlineStr"/>
       <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
+      <c r="H10" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: R104
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="60" customHeight="1">
       <c r="A11" s="6" t="inlineStr">
         <is>
-          <t>C2
-(15:00-17:00)</t>
+          <t>T1
+(17:30-19:30)</t>
         </is>
       </c>
       <c r="B11" s="7" t="inlineStr">
@@ -4158,36 +4417,66 @@
       <c r="C11" s="7" t="inlineStr"/>
       <c r="D11" s="7" t="inlineStr"/>
       <c r="E11" s="7" t="inlineStr"/>
-      <c r="F11" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Thiết kế Web
-Phòng: LAB01
-(Thực hành)</t>
+      <c r="F11" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Thiết kế Web
+Phòng: R104
+(Lý thuyết)</t>
         </is>
       </c>
       <c r="G11" s="7" t="inlineStr"/>
       <c r="H11" s="7" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" s="10" t="n"/>
+      <c r="A12" s="9" t="n"/>
       <c r="B12" s="7" t="inlineStr">
         <is>
           <t>Phạm Văn D</t>
         </is>
       </c>
-      <c r="C12" s="7" t="inlineStr"/>
+      <c r="C12" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Mạng máy tính
+Phòng: R101
+(Lý thuyết)</t>
+        </is>
+      </c>
       <c r="D12" s="7" t="inlineStr"/>
-      <c r="E12" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL04
-Môn: Mạng máy tính
-Phòng: R102
-(Lý thuyết)</t>
+      <c r="E12" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL04
+Môn: Mạng máy tính
+Phòng: LAB01
+(Thực hành)</t>
         </is>
       </c>
       <c r="F12" s="7" t="inlineStr"/>
-      <c r="G12" s="8" t="inlineStr">
+      <c r="G12" s="10" t="inlineStr">
+        <is>
+          <t>Lớp: CL03
+Môn: Thiết kế Web
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13" ht="60" customHeight="1">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>T2
+(19:30-21:30)</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>Phạm Văn D</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="inlineStr"/>
+      <c r="D13" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL03
 Môn: Mạng máy tính
@@ -4195,14 +4484,10 @@
 (Thực hành)</t>
         </is>
       </c>
-      <c r="H12" s="9" t="inlineStr">
-        <is>
-          <t>Lớp: CL03
-Môn: Mạng máy tính
-Phòng: R102
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="E13" s="7" t="inlineStr"/>
+      <c r="F13" s="7" t="inlineStr"/>
+      <c r="G13" s="7" t="inlineStr"/>
+      <c r="H13" s="7" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>